<commit_message>
fix: Change the way getting yesterday start, end and previous week start, end dates
</commit_message>
<xml_diff>
--- a/xlsx/2023/1/2023-02-20~2023-02-26.xlsx
+++ b/xlsx/2023/1/2023-02-20~2023-02-26.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="86">
   <si>
     <t>보행자 알림이 보고서</t>
   </si>
@@ -79,19 +79,19 @@
     <t>07 ~ 08</t>
   </si>
   <si>
-    <t>보행자 통행량 : 116086</t>
+    <t>보행자 통행량 : 18816</t>
   </si>
   <si>
     <t>보행자 통행량</t>
   </si>
   <si>
-    <t>차량 통행량: 151300</t>
+    <t>차량 통행량: 24291</t>
   </si>
   <si>
     <t>차량 통행량</t>
   </si>
   <si>
-    <t>불법주정차 수: 162</t>
+    <t>불법주정차 수: 16</t>
   </si>
   <si>
     <t>불법주정차 수</t>
@@ -148,130 +148,127 @@
     <t>개소 1</t>
   </si>
   <si>
-    <t>보행자 점유율 평균: 8.6</t>
+    <t>보행자 점유율 평균: 8.7</t>
   </si>
   <si>
     <t>보행자 점유율 평균</t>
   </si>
   <si>
-    <t>차량 통행량: 4457</t>
+    <t>차량 통행량: 632</t>
   </si>
   <si>
     <t>개소 2</t>
   </si>
   <si>
-    <t>보행자 통행량: 11412</t>
+    <t>보행자 통행량: 1702</t>
   </si>
   <si>
-    <t>차량 통행량: 4195</t>
+    <t>차량 통행량: 503</t>
   </si>
   <si>
     <t>개소 3</t>
   </si>
   <si>
-    <t>보행자 점유율 평균: 4.6</t>
+    <t>보행자 점유율 평균: 5.8</t>
   </si>
   <si>
-    <t>차량 통행량: 3690</t>
+    <t>차량 통행량: 575</t>
   </si>
   <si>
     <t>개소 4</t>
   </si>
   <si>
-    <t>보행자 점유율 평균: 2.7</t>
+    <t>보행자 점유율 평균: 2.6</t>
   </si>
   <si>
-    <t>차량 통행량: 2308</t>
+    <t>차량 통행량: 320</t>
   </si>
   <si>
     <t>개소 5</t>
   </si>
   <si>
-    <t>보행자 통행량: 11726</t>
+    <t>보행자 통행량: 2201</t>
   </si>
   <si>
-    <t>차량 통행량: 4597</t>
+    <t>차량 통행량: 673</t>
   </si>
   <si>
-    <t>불법주정차 수: 58</t>
+    <t>불법주정차 수: 10</t>
   </si>
   <si>
     <t>개소 6</t>
   </si>
   <si>
-    <t>보행자 통행량: 31228</t>
+    <t>보행자 통행량: 4283</t>
   </si>
   <si>
-    <t>차량 통행량: 2394</t>
+    <t>차량 통행량: 319</t>
   </si>
   <si>
-    <t>불법주정차 수: 104</t>
+    <t>불법주정차 수: 6</t>
   </si>
   <si>
     <t>개소 7</t>
   </si>
   <si>
-    <t>보행자 통행량: 23713</t>
+    <t>보행자 통행량: 3903</t>
   </si>
   <si>
-    <t>차량 통행량: 17058</t>
+    <t>차량 통행량: 2377</t>
   </si>
   <si>
     <t>개소 8</t>
   </si>
   <si>
-    <t>보행자 통행량: 22193</t>
+    <t>보행자 통행량: 3691</t>
   </si>
   <si>
-    <t>차량 통행량: 23295</t>
+    <t>차량 통행량: 3417</t>
   </si>
   <si>
     <t>개소 9</t>
   </si>
   <si>
-    <t>보행자 통행량: 3283</t>
+    <t>보행자 통행량: 518</t>
   </si>
   <si>
     <t>행자 통행량</t>
   </si>
   <si>
-    <t>차량 통행량: 3674</t>
+    <t>차량 통행량: 653</t>
   </si>
   <si>
     <t>개소 10</t>
   </si>
   <si>
-    <t>보행자 통행량: 5713</t>
+    <t>보행자 통행량: 886</t>
   </si>
   <si>
-    <t>차량 통행량: 23032</t>
+    <t>차량 통행량: 3387</t>
   </si>
   <si>
     <t>개소 11</t>
   </si>
   <si>
-    <t>보행자 통행량: 3988</t>
+    <t>보행자 통행량: 784</t>
   </si>
   <si>
-    <t>차량 통행량: 23985</t>
+    <t>차량 통행량: 3574</t>
   </si>
   <si>
     <t>개소 12</t>
   </si>
   <si>
-    <t>보행자 통행량: 1554</t>
-  </si>
-  <si>
-    <t>차량 통행량: 16289</t>
+    <t>보행자 통행량: 179</t>
   </si>
   <si>
     <t>개소 13</t>
   </si>
   <si>
-    <t>보행자 통행량: 1276</t>
+    <t>보행자 통행량: 669</t>
   </si>
   <si>
-    <t>차량 통행량: 22326</t>
+    <t>차량 통행량: 7358</t>
   </si>
 </sst>
 </file>
@@ -523,11 +520,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="275531203"/>
-        <c:axId val="279548820"/>
+        <c:axId val="1631124097"/>
+        <c:axId val="2143332592"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="275531203"/>
+        <c:axId val="1631124097"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -579,10 +576,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="279548820"/>
+        <c:crossAx val="2143332592"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="279548820"/>
+        <c:axId val="2143332592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -657,7 +654,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="275531203"/>
+        <c:crossAx val="1631124097"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -787,11 +784,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="951733203"/>
-        <c:axId val="2006187246"/>
+        <c:axId val="512271247"/>
+        <c:axId val="1638449719"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="951733203"/>
+        <c:axId val="512271247"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -843,10 +840,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2006187246"/>
+        <c:crossAx val="1638449719"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2006187246"/>
+        <c:axId val="1638449719"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -921,7 +918,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="951733203"/>
+        <c:crossAx val="512271247"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1051,11 +1048,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1725441547"/>
-        <c:axId val="1727867008"/>
+        <c:axId val="675920374"/>
+        <c:axId val="816481993"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1725441547"/>
+        <c:axId val="675920374"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1107,10 +1104,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1727867008"/>
+        <c:crossAx val="816481993"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1727867008"/>
+        <c:axId val="816481993"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1185,7 +1182,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1725441547"/>
+        <c:crossAx val="675920374"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1315,11 +1312,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="2018223539"/>
-        <c:axId val="10289415"/>
+        <c:axId val="22573025"/>
+        <c:axId val="178684283"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2018223539"/>
+        <c:axId val="22573025"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1371,10 +1368,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="10289415"/>
+        <c:crossAx val="178684283"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="10289415"/>
+        <c:axId val="178684283"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1449,7 +1446,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2018223539"/>
+        <c:crossAx val="22573025"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1579,11 +1576,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1936487751"/>
-        <c:axId val="1150057868"/>
+        <c:axId val="227414466"/>
+        <c:axId val="1596732555"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1936487751"/>
+        <c:axId val="227414466"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1635,10 +1632,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1150057868"/>
+        <c:crossAx val="1596732555"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1150057868"/>
+        <c:axId val="1596732555"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1713,7 +1710,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1936487751"/>
+        <c:crossAx val="227414466"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1843,11 +1840,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1235638425"/>
-        <c:axId val="215768683"/>
+        <c:axId val="220744837"/>
+        <c:axId val="1990215761"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1235638425"/>
+        <c:axId val="220744837"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1899,10 +1896,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="215768683"/>
+        <c:crossAx val="1990215761"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="215768683"/>
+        <c:axId val="1990215761"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1977,7 +1974,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1235638425"/>
+        <c:crossAx val="220744837"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2107,11 +2104,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1231404931"/>
-        <c:axId val="718433501"/>
+        <c:axId val="1751344934"/>
+        <c:axId val="540618331"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1231404931"/>
+        <c:axId val="1751344934"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2163,10 +2160,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="718433501"/>
+        <c:crossAx val="540618331"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="718433501"/>
+        <c:axId val="540618331"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2241,7 +2238,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1231404931"/>
+        <c:crossAx val="1751344934"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2371,11 +2368,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="558749574"/>
-        <c:axId val="135969439"/>
+        <c:axId val="43669538"/>
+        <c:axId val="29541877"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="558749574"/>
+        <c:axId val="43669538"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2427,10 +2424,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="135969439"/>
+        <c:crossAx val="29541877"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="135969439"/>
+        <c:axId val="29541877"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2505,7 +2502,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="558749574"/>
+        <c:crossAx val="43669538"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2684,11 +2681,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="429651485"/>
-        <c:axId val="1980365913"/>
+        <c:axId val="1478784687"/>
+        <c:axId val="912837828"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="429651485"/>
+        <c:axId val="1478784687"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2740,10 +2737,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1980365913"/>
+        <c:crossAx val="912837828"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1980365913"/>
+        <c:axId val="912837828"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2818,7 +2815,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="429651485"/>
+        <c:crossAx val="1478784687"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2997,11 +2994,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1099230619"/>
-        <c:axId val="131878856"/>
+        <c:axId val="1111766382"/>
+        <c:axId val="1929725972"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1099230619"/>
+        <c:axId val="1111766382"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3053,10 +3050,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="131878856"/>
+        <c:crossAx val="1929725972"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="131878856"/>
+        <c:axId val="1929725972"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3131,7 +3128,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1099230619"/>
+        <c:crossAx val="1111766382"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -3261,11 +3258,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1933707813"/>
-        <c:axId val="760238375"/>
+        <c:axId val="212491166"/>
+        <c:axId val="1655009309"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1933707813"/>
+        <c:axId val="212491166"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3317,10 +3314,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="760238375"/>
+        <c:crossAx val="1655009309"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="760238375"/>
+        <c:axId val="1655009309"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3395,7 +3392,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1933707813"/>
+        <c:crossAx val="212491166"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -3525,11 +3522,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1569950248"/>
-        <c:axId val="586213471"/>
+        <c:axId val="1934232065"/>
+        <c:axId val="1921267322"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1569950248"/>
+        <c:axId val="1934232065"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3581,10 +3578,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="586213471"/>
+        <c:crossAx val="1921267322"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="586213471"/>
+        <c:axId val="1921267322"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3659,7 +3656,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1569950248"/>
+        <c:crossAx val="1934232065"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -3789,11 +3786,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="859970192"/>
-        <c:axId val="1947302853"/>
+        <c:axId val="599863136"/>
+        <c:axId val="929867318"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="859970192"/>
+        <c:axId val="599863136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3845,10 +3842,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1947302853"/>
+        <c:crossAx val="929867318"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1947302853"/>
+        <c:axId val="929867318"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3923,7 +3920,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="859970192"/>
+        <c:crossAx val="599863136"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -4613,28 +4610,28 @@
         <v>23</v>
       </c>
       <c r="E11" s="11">
-        <v>828.0</v>
+        <v>128.0</v>
       </c>
       <c r="F11" s="11">
-        <v>425.0</v>
+        <v>53.0</v>
       </c>
       <c r="G11" s="11">
-        <v>237.0</v>
+        <v>39.0</v>
       </c>
       <c r="H11" s="11">
-        <v>234.0</v>
+        <v>47.0</v>
       </c>
       <c r="I11" s="11">
-        <v>650.0</v>
+        <v>143.0</v>
       </c>
       <c r="J11" s="11">
-        <v>1137.0</v>
+        <v>221.0</v>
       </c>
       <c r="K11" s="11">
-        <v>1661.0</v>
+        <v>328.0</v>
       </c>
       <c r="L11" s="11">
-        <v>3762.0</v>
+        <v>906.0</v>
       </c>
     </row>
     <row r="12">
@@ -4646,28 +4643,28 @@
         <v>25</v>
       </c>
       <c r="E12" s="11">
-        <v>2098.0</v>
+        <v>271.0</v>
       </c>
       <c r="F12" s="11">
-        <v>1534.0</v>
+        <v>167.0</v>
       </c>
       <c r="G12" s="11">
-        <v>1111.0</v>
+        <v>135.0</v>
       </c>
       <c r="H12" s="11">
-        <v>885.0</v>
+        <v>102.0</v>
       </c>
       <c r="I12" s="11">
-        <v>1150.0</v>
+        <v>206.0</v>
       </c>
       <c r="J12" s="11">
-        <v>2163.0</v>
+        <v>442.0</v>
       </c>
       <c r="K12" s="11">
-        <v>3584.0</v>
+        <v>810.0</v>
       </c>
       <c r="L12" s="11">
-        <v>5756.0</v>
+        <v>1271.0</v>
       </c>
     </row>
     <row r="13">
@@ -4679,28 +4676,28 @@
         <v>27</v>
       </c>
       <c r="E13" s="11">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="F13" s="11">
+        <v>0.0</v>
+      </c>
+      <c r="G13" s="11">
+        <v>0.0</v>
+      </c>
+      <c r="H13" s="11">
+        <v>0.0</v>
+      </c>
+      <c r="I13" s="11">
         <v>1.0</v>
       </c>
-      <c r="G13" s="11">
-        <v>2.0</v>
-      </c>
-      <c r="H13" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="I13" s="11">
+      <c r="J13" s="11">
         <v>0.0</v>
-      </c>
-      <c r="J13" s="11">
-        <v>1.0</v>
       </c>
       <c r="K13" s="11">
         <v>0.0</v>
       </c>
       <c r="L13" s="11">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="14">
@@ -4733,82 +4730,82 @@
     <row r="15">
       <c r="B15" s="13"/>
       <c r="E15" s="11">
-        <v>9056.0</v>
+        <v>1792.0</v>
       </c>
       <c r="F15" s="11">
-        <v>6883.0</v>
+        <v>1125.0</v>
       </c>
       <c r="G15" s="11">
-        <v>6643.0</v>
+        <v>932.0</v>
       </c>
       <c r="H15" s="11">
-        <v>6841.0</v>
+        <v>959.0</v>
       </c>
       <c r="I15" s="11">
-        <v>8483.0</v>
+        <v>1040.0</v>
       </c>
       <c r="J15" s="11">
-        <v>8208.0</v>
+        <v>1084.0</v>
       </c>
       <c r="K15" s="11">
-        <v>7653.0</v>
+        <v>1044.0</v>
       </c>
       <c r="L15" s="11">
-        <v>8178.0</v>
+        <v>1155.0</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" s="13"/>
       <c r="E16" s="11">
-        <v>10225.0</v>
+        <v>1926.0</v>
       </c>
       <c r="F16" s="11">
-        <v>10232.0</v>
+        <v>1698.0</v>
       </c>
       <c r="G16" s="11">
-        <v>9608.0</v>
+        <v>1440.0</v>
       </c>
       <c r="H16" s="11">
-        <v>8794.0</v>
+        <v>1279.0</v>
       </c>
       <c r="I16" s="11">
-        <v>8461.0</v>
+        <v>1134.0</v>
       </c>
       <c r="J16" s="11">
-        <v>8968.0</v>
+        <v>1206.0</v>
       </c>
       <c r="K16" s="11">
-        <v>9503.0</v>
+        <v>1427.0</v>
       </c>
       <c r="L16" s="11">
-        <v>10164.0</v>
+        <v>1488.0</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" s="13"/>
       <c r="E17" s="11">
-        <v>7.0</v>
+        <v>0.0</v>
       </c>
       <c r="F17" s="11">
-        <v>9.0</v>
+        <v>1.0</v>
       </c>
       <c r="G17" s="11">
-        <v>10.0</v>
+        <v>3.0</v>
       </c>
       <c r="H17" s="11">
-        <v>10.0</v>
+        <v>0.0</v>
       </c>
       <c r="I17" s="11">
-        <v>10.0</v>
+        <v>0.0</v>
       </c>
       <c r="J17" s="11">
-        <v>12.0</v>
+        <v>2.0</v>
       </c>
       <c r="K17" s="11">
-        <v>13.0</v>
+        <v>1.0</v>
       </c>
       <c r="L17" s="11">
-        <v>7.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="18">
@@ -4841,82 +4838,82 @@
     <row r="19">
       <c r="B19" s="13"/>
       <c r="E19" s="11">
-        <v>8422.0</v>
+        <v>1304.0</v>
       </c>
       <c r="F19" s="11">
-        <v>8591.0</v>
+        <v>1533.0</v>
       </c>
       <c r="G19" s="11">
-        <v>7756.0</v>
+        <v>1631.0</v>
       </c>
       <c r="H19" s="11">
-        <v>6550.0</v>
+        <v>1030.0</v>
       </c>
       <c r="I19" s="11">
-        <v>4984.0</v>
+        <v>849.0</v>
       </c>
       <c r="J19" s="11">
-        <v>4084.0</v>
+        <v>686.0</v>
       </c>
       <c r="K19" s="11">
-        <v>3155.0</v>
+        <v>508.0</v>
       </c>
       <c r="L19" s="11">
-        <v>1665.0</v>
+        <v>279.0</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" s="13"/>
       <c r="E20" s="11">
-        <v>10898.0</v>
+        <v>1659.0</v>
       </c>
       <c r="F20" s="11">
-        <v>11201.0</v>
+        <v>1878.0</v>
       </c>
       <c r="G20" s="11">
-        <v>10514.0</v>
+        <v>1887.0</v>
       </c>
       <c r="H20" s="11">
-        <v>7747.0</v>
+        <v>1242.0</v>
       </c>
       <c r="I20" s="11">
-        <v>5739.0</v>
+        <v>882.0</v>
       </c>
       <c r="J20" s="11">
-        <v>4618.0</v>
+        <v>732.0</v>
       </c>
       <c r="K20" s="11">
-        <v>3761.0</v>
+        <v>595.0</v>
       </c>
       <c r="L20" s="11">
-        <v>2586.0</v>
+        <v>414.0</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" s="13"/>
       <c r="E21" s="11">
-        <v>14.0</v>
+        <v>0.0</v>
       </c>
       <c r="F21" s="11">
-        <v>16.0</v>
+        <v>3.0</v>
       </c>
       <c r="G21" s="11">
-        <v>13.0</v>
+        <v>1.0</v>
       </c>
       <c r="H21" s="11">
-        <v>7.0</v>
+        <v>1.0</v>
       </c>
       <c r="I21" s="11">
-        <v>9.0</v>
+        <v>1.0</v>
       </c>
       <c r="J21" s="11">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="K21" s="11">
-        <v>6.0</v>
+        <v>1.0</v>
       </c>
       <c r="L21" s="11">
-        <v>6.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="22">
@@ -4963,28 +4960,28 @@
         <v>46</v>
       </c>
       <c r="E23" s="11">
-        <v>2.1</v>
+        <v>2.0</v>
       </c>
       <c r="F23" s="11">
-        <v>1.3</v>
+        <v>0.7</v>
       </c>
       <c r="G23" s="11">
-        <v>0.7</v>
+        <v>1.0</v>
       </c>
       <c r="H23" s="11">
-        <v>0.7</v>
+        <v>1.0</v>
       </c>
       <c r="I23" s="11">
-        <v>1.1</v>
+        <v>1.0</v>
       </c>
       <c r="J23" s="11">
-        <v>2.7</v>
+        <v>3.3</v>
       </c>
       <c r="K23" s="11">
-        <v>3.5</v>
+        <v>5.0</v>
       </c>
       <c r="L23" s="11">
-        <v>4.4</v>
+        <v>7.7</v>
       </c>
     </row>
     <row r="24">
@@ -4996,28 +4993,28 @@
         <v>25</v>
       </c>
       <c r="E24" s="11">
-        <v>75.0</v>
+        <v>5.0</v>
       </c>
       <c r="F24" s="11">
-        <v>108.0</v>
+        <v>2.0</v>
       </c>
       <c r="G24" s="11">
-        <v>61.0</v>
+        <v>2.0</v>
       </c>
       <c r="H24" s="11">
-        <v>33.0</v>
+        <v>1.0</v>
       </c>
       <c r="I24" s="11">
-        <v>29.0</v>
+        <v>8.0</v>
       </c>
       <c r="J24" s="11">
-        <v>68.0</v>
+        <v>13.0</v>
       </c>
       <c r="K24" s="11">
-        <v>111.0</v>
+        <v>19.0</v>
       </c>
       <c r="L24" s="11">
-        <v>157.0</v>
+        <v>32.0</v>
       </c>
     </row>
     <row r="25">
@@ -5063,55 +5060,55 @@
     <row r="27">
       <c r="B27" s="13"/>
       <c r="E27" s="11">
-        <v>7.7</v>
+        <v>10.0</v>
       </c>
       <c r="F27" s="11">
-        <v>10.1</v>
+        <v>11.0</v>
       </c>
       <c r="G27" s="11">
-        <v>19.3</v>
+        <v>16.3</v>
       </c>
       <c r="H27" s="11">
-        <v>13.4</v>
+        <v>10.7</v>
       </c>
       <c r="I27" s="11">
-        <v>13.6</v>
+        <v>10.7</v>
       </c>
       <c r="J27" s="11">
-        <v>12.4</v>
+        <v>15.0</v>
       </c>
       <c r="K27" s="11">
-        <v>15.9</v>
+        <v>12.3</v>
       </c>
       <c r="L27" s="11">
-        <v>16.3</v>
+        <v>24.3</v>
       </c>
     </row>
     <row r="28">
       <c r="B28" s="13"/>
       <c r="E28" s="11">
-        <v>216.0</v>
+        <v>41.0</v>
       </c>
       <c r="F28" s="11">
-        <v>272.0</v>
+        <v>48.0</v>
       </c>
       <c r="G28" s="11">
-        <v>252.0</v>
+        <v>39.0</v>
       </c>
       <c r="H28" s="11">
-        <v>297.0</v>
+        <v>39.0</v>
       </c>
       <c r="I28" s="11">
-        <v>246.0</v>
+        <v>25.0</v>
       </c>
       <c r="J28" s="11">
-        <v>252.0</v>
+        <v>36.0</v>
       </c>
       <c r="K28" s="11">
-        <v>296.0</v>
+        <v>41.0</v>
       </c>
       <c r="L28" s="11">
-        <v>292.0</v>
+        <v>30.0</v>
       </c>
     </row>
     <row r="29">
@@ -5155,25 +5152,25 @@
     <row r="31">
       <c r="B31" s="13"/>
       <c r="E31" s="11">
-        <v>18.7</v>
+        <v>15.0</v>
       </c>
       <c r="F31" s="11">
-        <v>14.6</v>
+        <v>14.7</v>
       </c>
       <c r="G31" s="11">
-        <v>13.1</v>
+        <v>14.0</v>
       </c>
       <c r="H31" s="11">
-        <v>11.6</v>
+        <v>10.0</v>
       </c>
       <c r="I31" s="11">
-        <v>7.7</v>
+        <v>8.0</v>
       </c>
       <c r="J31" s="11">
-        <v>6.9</v>
+        <v>8.3</v>
       </c>
       <c r="K31" s="11">
-        <v>6.3</v>
+        <v>3.3</v>
       </c>
       <c r="L31" s="11">
         <v>3.0</v>
@@ -5182,28 +5179,28 @@
     <row r="32">
       <c r="B32" s="13"/>
       <c r="E32" s="11">
-        <v>330.0</v>
+        <v>50.0</v>
       </c>
       <c r="F32" s="11">
-        <v>317.0</v>
+        <v>64.0</v>
       </c>
       <c r="G32" s="11">
-        <v>305.0</v>
+        <v>51.0</v>
       </c>
       <c r="H32" s="11">
-        <v>233.0</v>
+        <v>33.0</v>
       </c>
       <c r="I32" s="11">
-        <v>168.0</v>
+        <v>18.0</v>
       </c>
       <c r="J32" s="11">
-        <v>143.0</v>
+        <v>20.0</v>
       </c>
       <c r="K32" s="11">
-        <v>118.0</v>
+        <v>6.0</v>
       </c>
       <c r="L32" s="11">
-        <v>78.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="33">
@@ -5261,28 +5258,28 @@
         <v>23</v>
       </c>
       <c r="E35" s="11">
-        <v>148.0</v>
+        <v>17.0</v>
       </c>
       <c r="F35" s="11">
-        <v>95.0</v>
+        <v>7.0</v>
       </c>
       <c r="G35" s="11">
-        <v>44.0</v>
+        <v>8.0</v>
       </c>
       <c r="H35" s="11">
-        <v>36.0</v>
+        <v>5.0</v>
       </c>
       <c r="I35" s="11">
-        <v>61.0</v>
+        <v>22.0</v>
       </c>
       <c r="J35" s="11">
-        <v>133.0</v>
+        <v>16.0</v>
       </c>
       <c r="K35" s="11">
-        <v>159.0</v>
+        <v>31.0</v>
       </c>
       <c r="L35" s="11">
-        <v>352.0</v>
+        <v>75.0</v>
       </c>
     </row>
     <row r="36">
@@ -5294,28 +5291,28 @@
         <v>25</v>
       </c>
       <c r="E36" s="11">
-        <v>33.0</v>
+        <v>2.0</v>
       </c>
       <c r="F36" s="11">
-        <v>44.0</v>
+        <v>3.0</v>
       </c>
       <c r="G36" s="11">
-        <v>45.0</v>
+        <v>3.0</v>
       </c>
       <c r="H36" s="11">
-        <v>14.0</v>
+        <v>4.0</v>
       </c>
       <c r="I36" s="11">
-        <v>39.0</v>
+        <v>2.0</v>
       </c>
       <c r="J36" s="11">
-        <v>72.0</v>
+        <v>11.0</v>
       </c>
       <c r="K36" s="11">
-        <v>113.0</v>
+        <v>24.0</v>
       </c>
       <c r="L36" s="11">
-        <v>192.0</v>
+        <v>38.0</v>
       </c>
     </row>
     <row r="37">
@@ -5361,55 +5358,55 @@
     <row r="39">
       <c r="B39" s="13"/>
       <c r="E39" s="11">
-        <v>732.0</v>
+        <v>109.0</v>
       </c>
       <c r="F39" s="11">
-        <v>613.0</v>
+        <v>79.0</v>
       </c>
       <c r="G39" s="11">
-        <v>626.0</v>
+        <v>75.0</v>
       </c>
       <c r="H39" s="11">
-        <v>739.0</v>
+        <v>97.0</v>
       </c>
       <c r="I39" s="11">
-        <v>765.0</v>
+        <v>95.0</v>
       </c>
       <c r="J39" s="11">
-        <v>727.0</v>
+        <v>106.0</v>
       </c>
       <c r="K39" s="11">
-        <v>773.0</v>
+        <v>108.0</v>
       </c>
       <c r="L39" s="11">
-        <v>757.0</v>
+        <v>115.0</v>
       </c>
     </row>
     <row r="40">
       <c r="B40" s="13"/>
       <c r="E40" s="11">
-        <v>466.0</v>
+        <v>60.0</v>
       </c>
       <c r="F40" s="11">
-        <v>301.0</v>
+        <v>18.0</v>
       </c>
       <c r="G40" s="11">
-        <v>292.0</v>
+        <v>24.0</v>
       </c>
       <c r="H40" s="11">
-        <v>243.0</v>
+        <v>17.0</v>
       </c>
       <c r="I40" s="11">
-        <v>266.0</v>
+        <v>22.0</v>
       </c>
       <c r="J40" s="11">
-        <v>245.0</v>
+        <v>22.0</v>
       </c>
       <c r="K40" s="11">
-        <v>237.0</v>
+        <v>30.0</v>
       </c>
       <c r="L40" s="11">
-        <v>260.0</v>
+        <v>41.0</v>
       </c>
     </row>
     <row r="41">
@@ -5453,55 +5450,55 @@
     <row r="43">
       <c r="B43" s="13"/>
       <c r="E43" s="11">
-        <v>756.0</v>
+        <v>118.0</v>
       </c>
       <c r="F43" s="11">
-        <v>821.0</v>
+        <v>128.0</v>
       </c>
       <c r="G43" s="11">
-        <v>760.0</v>
+        <v>122.0</v>
       </c>
       <c r="H43" s="11">
-        <v>696.0</v>
+        <v>134.0</v>
       </c>
       <c r="I43" s="11">
-        <v>588.0</v>
+        <v>95.0</v>
       </c>
       <c r="J43" s="11">
-        <v>488.0</v>
+        <v>58.0</v>
       </c>
       <c r="K43" s="11">
-        <v>382.0</v>
+        <v>62.0</v>
       </c>
       <c r="L43" s="11">
-        <v>161.0</v>
+        <v>20.0</v>
       </c>
     </row>
     <row r="44">
       <c r="B44" s="13"/>
       <c r="E44" s="11">
-        <v>258.0</v>
+        <v>42.0</v>
       </c>
       <c r="F44" s="11">
-        <v>281.0</v>
+        <v>36.0</v>
       </c>
       <c r="G44" s="11">
-        <v>233.0</v>
+        <v>40.0</v>
       </c>
       <c r="H44" s="11">
-        <v>189.0</v>
+        <v>28.0</v>
       </c>
       <c r="I44" s="11">
-        <v>135.0</v>
+        <v>14.0</v>
       </c>
       <c r="J44" s="11">
-        <v>131.0</v>
+        <v>15.0</v>
       </c>
       <c r="K44" s="11">
-        <v>59.0</v>
+        <v>4.0</v>
       </c>
       <c r="L44" s="11">
-        <v>47.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="45">
@@ -5559,28 +5556,28 @@
         <v>46</v>
       </c>
       <c r="E47" s="11">
-        <v>0.9</v>
+        <v>1.0</v>
       </c>
       <c r="F47" s="11">
-        <v>0.8</v>
+        <v>1.0</v>
       </c>
       <c r="G47" s="11">
+        <v>0.0</v>
+      </c>
+      <c r="H47" s="11">
         <v>0.3</v>
       </c>
-      <c r="H47" s="11">
-        <v>0.4</v>
-      </c>
       <c r="I47" s="11">
-        <v>0.5</v>
+        <v>1.0</v>
       </c>
       <c r="J47" s="11">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="K47" s="11">
-        <v>1.6</v>
+        <v>2.0</v>
       </c>
       <c r="L47" s="11">
-        <v>2.7</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="48">
@@ -5592,28 +5589,28 @@
         <v>25</v>
       </c>
       <c r="E48" s="11">
-        <v>46.0</v>
+        <v>8.0</v>
       </c>
       <c r="F48" s="11">
-        <v>37.0</v>
+        <v>4.0</v>
       </c>
       <c r="G48" s="11">
-        <v>19.0</v>
+        <v>3.0</v>
       </c>
       <c r="H48" s="11">
-        <v>19.0</v>
+        <v>5.0</v>
       </c>
       <c r="I48" s="11">
-        <v>32.0</v>
+        <v>6.0</v>
       </c>
       <c r="J48" s="11">
-        <v>54.0</v>
+        <v>5.0</v>
       </c>
       <c r="K48" s="11">
-        <v>74.0</v>
+        <v>17.0</v>
       </c>
       <c r="L48" s="11">
-        <v>152.0</v>
+        <v>30.0</v>
       </c>
     </row>
     <row r="49">
@@ -5659,55 +5656,55 @@
     <row r="51">
       <c r="B51" s="13"/>
       <c r="E51" s="11">
-        <v>7.2</v>
+        <v>9.7</v>
       </c>
       <c r="F51" s="11">
-        <v>5.5</v>
+        <v>6.3</v>
       </c>
       <c r="G51" s="11">
-        <v>5.6</v>
+        <v>11.3</v>
       </c>
       <c r="H51" s="11">
-        <v>7.1</v>
+        <v>6.7</v>
       </c>
       <c r="I51" s="11">
-        <v>7.7</v>
+        <v>10.3</v>
       </c>
       <c r="J51" s="11">
-        <v>7.6</v>
+        <v>8.7</v>
       </c>
       <c r="K51" s="11">
-        <v>9.1</v>
+        <v>6.0</v>
       </c>
       <c r="L51" s="11">
-        <v>9.4</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="52">
       <c r="B52" s="13"/>
       <c r="E52" s="11">
-        <v>216.0</v>
+        <v>30.0</v>
       </c>
       <c r="F52" s="11">
-        <v>244.0</v>
+        <v>37.0</v>
       </c>
       <c r="G52" s="11">
-        <v>231.0</v>
+        <v>35.0</v>
       </c>
       <c r="H52" s="11">
-        <v>238.0</v>
+        <v>33.0</v>
       </c>
       <c r="I52" s="11">
-        <v>234.0</v>
+        <v>38.0</v>
       </c>
       <c r="J52" s="11">
-        <v>199.0</v>
+        <v>27.0</v>
       </c>
       <c r="K52" s="11">
-        <v>255.0</v>
+        <v>34.0</v>
       </c>
       <c r="L52" s="11">
-        <v>252.0</v>
+        <v>41.0</v>
       </c>
     </row>
     <row r="53">
@@ -5751,55 +5748,55 @@
     <row r="55">
       <c r="B55" s="13"/>
       <c r="E55" s="11">
-        <v>9.0</v>
+        <v>15.3</v>
       </c>
       <c r="F55" s="11">
-        <v>8.8</v>
+        <v>11.3</v>
       </c>
       <c r="G55" s="11">
-        <v>6.2</v>
+        <v>10.0</v>
       </c>
       <c r="H55" s="11">
-        <v>6.1</v>
+        <v>7.7</v>
       </c>
       <c r="I55" s="11">
-        <v>5.0</v>
+        <v>5.3</v>
       </c>
       <c r="J55" s="11">
-        <v>2.9</v>
+        <v>5.3</v>
       </c>
       <c r="K55" s="11">
-        <v>3.5</v>
+        <v>3.7</v>
       </c>
       <c r="L55" s="11">
-        <v>1.6</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="56">
       <c r="B56" s="13"/>
       <c r="E56" s="11">
-        <v>276.0</v>
+        <v>46.0</v>
       </c>
       <c r="F56" s="11">
-        <v>288.0</v>
+        <v>52.0</v>
       </c>
       <c r="G56" s="11">
-        <v>245.0</v>
+        <v>48.0</v>
       </c>
       <c r="H56" s="11">
-        <v>167.0</v>
+        <v>25.0</v>
       </c>
       <c r="I56" s="11">
-        <v>137.0</v>
+        <v>19.0</v>
       </c>
       <c r="J56" s="11">
-        <v>120.0</v>
+        <v>10.0</v>
       </c>
       <c r="K56" s="11">
-        <v>91.0</v>
+        <v>12.0</v>
       </c>
       <c r="L56" s="11">
-        <v>64.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="57">
@@ -5860,25 +5857,25 @@
         <v>0.7</v>
       </c>
       <c r="F59" s="11">
-        <v>0.4</v>
+        <v>0.7</v>
       </c>
       <c r="G59" s="11">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="H59" s="11">
         <v>0.0</v>
       </c>
       <c r="I59" s="11">
-        <v>0.2</v>
+        <v>0.0</v>
       </c>
       <c r="J59" s="11">
+        <v>0.3</v>
+      </c>
+      <c r="K59" s="11">
         <v>0.7</v>
       </c>
-      <c r="K59" s="11">
-        <v>1.8</v>
-      </c>
       <c r="L59" s="11">
-        <v>3.6</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="60">
@@ -5890,28 +5887,28 @@
         <v>25</v>
       </c>
       <c r="E60" s="11">
-        <v>17.0</v>
+        <v>0.0</v>
       </c>
       <c r="F60" s="11">
-        <v>17.0</v>
+        <v>1.0</v>
       </c>
       <c r="G60" s="11">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
       <c r="H60" s="11">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="I60" s="11">
         <v>0.0</v>
       </c>
       <c r="J60" s="11">
-        <v>9.0</v>
+        <v>1.0</v>
       </c>
       <c r="K60" s="11">
-        <v>24.0</v>
+        <v>3.0</v>
       </c>
       <c r="L60" s="11">
-        <v>88.0</v>
+        <v>14.0</v>
       </c>
     </row>
     <row r="61">
@@ -5957,55 +5954,55 @@
     <row r="63">
       <c r="B63" s="13"/>
       <c r="E63" s="11">
-        <v>2.3</v>
+        <v>3.0</v>
       </c>
       <c r="F63" s="11">
-        <v>3.2</v>
+        <v>3.0</v>
       </c>
       <c r="G63" s="11">
-        <v>4.4</v>
+        <v>1.8</v>
       </c>
       <c r="H63" s="11">
-        <v>4.6</v>
+        <v>2.1</v>
       </c>
       <c r="I63" s="11">
-        <v>5.2</v>
+        <v>3.3</v>
       </c>
       <c r="J63" s="11">
-        <v>3.5</v>
+        <v>4.7</v>
       </c>
       <c r="K63" s="11">
-        <v>4.3</v>
+        <v>2.5</v>
       </c>
       <c r="L63" s="11">
-        <v>5.3</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="64">
       <c r="B64" s="13"/>
       <c r="E64" s="11">
-        <v>215.0</v>
+        <v>37.0</v>
       </c>
       <c r="F64" s="11">
-        <v>170.0</v>
+        <v>24.0</v>
       </c>
       <c r="G64" s="11">
-        <v>157.0</v>
+        <v>32.0</v>
       </c>
       <c r="H64" s="11">
-        <v>151.0</v>
+        <v>19.0</v>
       </c>
       <c r="I64" s="11">
-        <v>155.0</v>
+        <v>17.0</v>
       </c>
       <c r="J64" s="11">
-        <v>167.0</v>
+        <v>16.0</v>
       </c>
       <c r="K64" s="11">
-        <v>155.0</v>
+        <v>24.0</v>
       </c>
       <c r="L64" s="11">
-        <v>183.0</v>
+        <v>26.0</v>
       </c>
     </row>
     <row r="65">
@@ -6049,55 +6046,55 @@
     <row r="67">
       <c r="B67" s="13"/>
       <c r="E67" s="11">
-        <v>4.5</v>
+        <v>7.3</v>
       </c>
       <c r="F67" s="11">
-        <v>3.8</v>
+        <v>3.7</v>
       </c>
       <c r="G67" s="11">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="H67" s="11">
-        <v>4.6</v>
+        <v>3.7</v>
       </c>
       <c r="I67" s="11">
-        <v>2.4</v>
+        <v>4.3</v>
       </c>
       <c r="J67" s="11">
-        <v>2.1</v>
+        <v>2.0</v>
       </c>
       <c r="K67" s="11">
-        <v>3.3</v>
+        <v>1.3</v>
       </c>
       <c r="L67" s="11">
-        <v>1.2</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="68">
       <c r="B68" s="13"/>
       <c r="E68" s="11">
-        <v>205.0</v>
+        <v>21.0</v>
       </c>
       <c r="F68" s="11">
-        <v>236.0</v>
+        <v>34.0</v>
       </c>
       <c r="G68" s="11">
-        <v>105.0</v>
+        <v>32.0</v>
       </c>
       <c r="H68" s="11">
-        <v>76.0</v>
+        <v>9.0</v>
       </c>
       <c r="I68" s="11">
-        <v>60.0</v>
+        <v>6.0</v>
       </c>
       <c r="J68" s="11">
-        <v>52.0</v>
+        <v>1.0</v>
       </c>
       <c r="K68" s="11">
-        <v>31.0</v>
+        <v>1.0</v>
       </c>
       <c r="L68" s="11">
-        <v>26.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="69">
@@ -6155,28 +6152,28 @@
         <v>23</v>
       </c>
       <c r="E71" s="11">
-        <v>100.0</v>
+        <v>15.0</v>
       </c>
       <c r="F71" s="11">
-        <v>33.0</v>
+        <v>7.0</v>
       </c>
       <c r="G71" s="11">
-        <v>21.0</v>
+        <v>7.0</v>
       </c>
       <c r="H71" s="11">
-        <v>15.0</v>
+        <v>5.0</v>
       </c>
       <c r="I71" s="11">
-        <v>140.0</v>
+        <v>41.0</v>
       </c>
       <c r="J71" s="11">
-        <v>280.0</v>
+        <v>74.0</v>
       </c>
       <c r="K71" s="11">
-        <v>220.0</v>
+        <v>64.0</v>
       </c>
       <c r="L71" s="11">
-        <v>336.0</v>
+        <v>94.0</v>
       </c>
     </row>
     <row r="72">
@@ -6188,28 +6185,28 @@
         <v>25</v>
       </c>
       <c r="E72" s="11">
-        <v>56.0</v>
+        <v>10.0</v>
       </c>
       <c r="F72" s="11">
-        <v>42.0</v>
+        <v>5.0</v>
       </c>
       <c r="G72" s="11">
-        <v>38.0</v>
+        <v>5.0</v>
       </c>
       <c r="H72" s="11">
-        <v>23.0</v>
+        <v>1.0</v>
       </c>
       <c r="I72" s="11">
-        <v>68.0</v>
+        <v>19.0</v>
       </c>
       <c r="J72" s="11">
-        <v>169.0</v>
+        <v>39.0</v>
       </c>
       <c r="K72" s="11">
-        <v>75.0</v>
+        <v>14.0</v>
       </c>
       <c r="L72" s="11">
-        <v>83.0</v>
+        <v>18.0</v>
       </c>
     </row>
     <row r="73">
@@ -6242,7 +6239,7 @@
         <v>0.0</v>
       </c>
       <c r="L73" s="11">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="74">
@@ -6275,82 +6272,82 @@
     <row r="75">
       <c r="B75" s="13"/>
       <c r="E75" s="11">
-        <v>755.0</v>
+        <v>157.0</v>
       </c>
       <c r="F75" s="11">
-        <v>615.0</v>
+        <v>134.0</v>
       </c>
       <c r="G75" s="11">
-        <v>605.0</v>
+        <v>122.0</v>
       </c>
       <c r="H75" s="11">
-        <v>649.0</v>
+        <v>108.0</v>
       </c>
       <c r="I75" s="11">
-        <v>624.0</v>
+        <v>115.0</v>
       </c>
       <c r="J75" s="11">
-        <v>816.0</v>
+        <v>148.0</v>
       </c>
       <c r="K75" s="11">
-        <v>959.0</v>
+        <v>123.0</v>
       </c>
       <c r="L75" s="11">
-        <v>873.0</v>
+        <v>172.0</v>
       </c>
     </row>
     <row r="76">
       <c r="B76" s="13"/>
       <c r="E76" s="11">
-        <v>158.0</v>
+        <v>30.0</v>
       </c>
       <c r="F76" s="11">
-        <v>218.0</v>
+        <v>44.0</v>
       </c>
       <c r="G76" s="11">
-        <v>274.0</v>
+        <v>56.0</v>
       </c>
       <c r="H76" s="11">
-        <v>299.0</v>
+        <v>36.0</v>
       </c>
       <c r="I76" s="11">
-        <v>240.0</v>
+        <v>45.0</v>
       </c>
       <c r="J76" s="11">
-        <v>317.0</v>
+        <v>28.0</v>
       </c>
       <c r="K76" s="11">
-        <v>326.0</v>
+        <v>36.0</v>
       </c>
       <c r="L76" s="11">
-        <v>346.0</v>
+        <v>64.0</v>
       </c>
     </row>
     <row r="77">
       <c r="B77" s="13"/>
       <c r="E77" s="11">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="F77" s="11">
         <v>1.0</v>
       </c>
       <c r="G77" s="11">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="H77" s="11">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="I77" s="11">
+        <v>0.0</v>
+      </c>
+      <c r="J77" s="11">
         <v>1.0</v>
       </c>
-      <c r="J77" s="11">
-        <v>3.0</v>
-      </c>
       <c r="K77" s="11">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="L77" s="11">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="78">
@@ -6383,82 +6380,82 @@
     <row r="79">
       <c r="B79" s="13"/>
       <c r="E79" s="11">
-        <v>977.0</v>
+        <v>203.0</v>
       </c>
       <c r="F79" s="11">
-        <v>929.0</v>
+        <v>217.0</v>
       </c>
       <c r="G79" s="11">
-        <v>850.0</v>
+        <v>141.0</v>
       </c>
       <c r="H79" s="11">
-        <v>782.0</v>
+        <v>104.0</v>
       </c>
       <c r="I79" s="11">
-        <v>443.0</v>
+        <v>73.0</v>
       </c>
       <c r="J79" s="11">
-        <v>315.0</v>
+        <v>32.0</v>
       </c>
       <c r="K79" s="11">
-        <v>226.0</v>
+        <v>27.0</v>
       </c>
       <c r="L79" s="11">
-        <v>163.0</v>
+        <v>18.0</v>
       </c>
     </row>
     <row r="80">
       <c r="B80" s="13"/>
       <c r="E80" s="11">
-        <v>410.0</v>
+        <v>52.0</v>
       </c>
       <c r="F80" s="11">
-        <v>366.0</v>
+        <v>74.0</v>
       </c>
       <c r="G80" s="11">
-        <v>384.0</v>
+        <v>40.0</v>
       </c>
       <c r="H80" s="11">
-        <v>263.0</v>
+        <v>24.0</v>
       </c>
       <c r="I80" s="11">
-        <v>157.0</v>
+        <v>11.0</v>
       </c>
       <c r="J80" s="11">
-        <v>117.0</v>
+        <v>13.0</v>
       </c>
       <c r="K80" s="11">
-        <v>88.0</v>
+        <v>4.0</v>
       </c>
       <c r="L80" s="11">
-        <v>80.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="81">
       <c r="B81" s="13"/>
       <c r="E81" s="11">
-        <v>9.0</v>
+        <v>0.0</v>
       </c>
       <c r="F81" s="11">
-        <v>8.0</v>
+        <v>1.0</v>
       </c>
       <c r="G81" s="11">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="H81" s="11">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="I81" s="11">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="J81" s="11">
         <v>0.0</v>
       </c>
       <c r="K81" s="11">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="L81" s="11">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="82">
@@ -6505,28 +6502,28 @@
         <v>23</v>
       </c>
       <c r="E83" s="11">
-        <v>82.0</v>
+        <v>8.0</v>
       </c>
       <c r="F83" s="11">
-        <v>39.0</v>
+        <v>5.0</v>
       </c>
       <c r="G83" s="11">
-        <v>26.0</v>
+        <v>3.0</v>
       </c>
       <c r="H83" s="11">
-        <v>43.0</v>
+        <v>8.0</v>
       </c>
       <c r="I83" s="11">
-        <v>160.0</v>
+        <v>33.0</v>
       </c>
       <c r="J83" s="11">
-        <v>247.0</v>
+        <v>25.0</v>
       </c>
       <c r="K83" s="11">
-        <v>216.0</v>
+        <v>35.0</v>
       </c>
       <c r="L83" s="11">
-        <v>550.0</v>
+        <v>151.0</v>
       </c>
     </row>
     <row r="84">
@@ -6538,28 +6535,28 @@
         <v>25</v>
       </c>
       <c r="E84" s="11">
-        <v>38.0</v>
+        <v>3.0</v>
       </c>
       <c r="F84" s="11">
-        <v>45.0</v>
+        <v>5.0</v>
       </c>
       <c r="G84" s="11">
-        <v>24.0</v>
+        <v>4.0</v>
       </c>
       <c r="H84" s="11">
-        <v>39.0</v>
+        <v>4.0</v>
       </c>
       <c r="I84" s="11">
-        <v>46.0</v>
+        <v>10.0</v>
       </c>
       <c r="J84" s="11">
-        <v>93.0</v>
+        <v>17.0</v>
       </c>
       <c r="K84" s="11">
-        <v>96.0</v>
+        <v>23.0</v>
       </c>
       <c r="L84" s="11">
-        <v>116.0</v>
+        <v>31.0</v>
       </c>
     </row>
     <row r="85">
@@ -6571,22 +6568,22 @@
         <v>27</v>
       </c>
       <c r="E85" s="11">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="F85" s="11">
+        <v>0.0</v>
+      </c>
+      <c r="G85" s="11">
+        <v>0.0</v>
+      </c>
+      <c r="H85" s="11">
+        <v>0.0</v>
+      </c>
+      <c r="I85" s="11">
         <v>1.0</v>
       </c>
-      <c r="G85" s="11">
-        <v>2.0</v>
-      </c>
-      <c r="H85" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="I85" s="11">
+      <c r="J85" s="11">
         <v>0.0</v>
-      </c>
-      <c r="J85" s="11">
-        <v>1.0</v>
       </c>
       <c r="K85" s="11">
         <v>0.0</v>
@@ -6625,82 +6622,82 @@
     <row r="87">
       <c r="B87" s="13"/>
       <c r="E87" s="11">
-        <v>1331.0</v>
+        <v>260.0</v>
       </c>
       <c r="F87" s="11">
-        <v>1746.0</v>
+        <v>298.0</v>
       </c>
       <c r="G87" s="11">
-        <v>2282.0</v>
+        <v>299.0</v>
       </c>
       <c r="H87" s="11">
-        <v>2217.0</v>
+        <v>290.0</v>
       </c>
       <c r="I87" s="11">
-        <v>2315.0</v>
+        <v>192.0</v>
       </c>
       <c r="J87" s="11">
-        <v>2519.0</v>
+        <v>260.0</v>
       </c>
       <c r="K87" s="11">
-        <v>2620.0</v>
+        <v>332.0</v>
       </c>
       <c r="L87" s="11">
-        <v>2816.0</v>
+        <v>339.0</v>
       </c>
     </row>
     <row r="88">
       <c r="B88" s="13"/>
       <c r="E88" s="11">
-        <v>174.0</v>
+        <v>23.0</v>
       </c>
       <c r="F88" s="11">
-        <v>152.0</v>
+        <v>22.0</v>
       </c>
       <c r="G88" s="11">
-        <v>146.0</v>
+        <v>27.0</v>
       </c>
       <c r="H88" s="11">
-        <v>150.0</v>
+        <v>15.0</v>
       </c>
       <c r="I88" s="11">
-        <v>158.0</v>
+        <v>15.0</v>
       </c>
       <c r="J88" s="11">
-        <v>126.0</v>
+        <v>14.0</v>
       </c>
       <c r="K88" s="11">
-        <v>113.0</v>
+        <v>16.0</v>
       </c>
       <c r="L88" s="11">
-        <v>129.0</v>
+        <v>18.0</v>
       </c>
     </row>
     <row r="89">
       <c r="B89" s="13"/>
       <c r="E89" s="11">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
       <c r="F89" s="11">
-        <v>8.0</v>
+        <v>0.0</v>
       </c>
       <c r="G89" s="11">
-        <v>6.0</v>
+        <v>0.0</v>
       </c>
       <c r="H89" s="11">
-        <v>6.0</v>
+        <v>0.0</v>
       </c>
       <c r="I89" s="11">
-        <v>9.0</v>
+        <v>0.0</v>
       </c>
       <c r="J89" s="11">
-        <v>9.0</v>
+        <v>1.0</v>
       </c>
       <c r="K89" s="11">
-        <v>8.0</v>
+        <v>0.0</v>
       </c>
       <c r="L89" s="11">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="90">
@@ -6733,82 +6730,82 @@
     <row r="91">
       <c r="B91" s="13"/>
       <c r="E91" s="11">
-        <v>2906.0</v>
+        <v>365.0</v>
       </c>
       <c r="F91" s="11">
-        <v>2589.0</v>
+        <v>372.0</v>
       </c>
       <c r="G91" s="11">
-        <v>2141.0</v>
+        <v>345.0</v>
       </c>
       <c r="H91" s="11">
-        <v>1650.0</v>
+        <v>311.0</v>
       </c>
       <c r="I91" s="11">
-        <v>1215.0</v>
+        <v>157.0</v>
       </c>
       <c r="J91" s="11">
-        <v>815.0</v>
+        <v>104.0</v>
       </c>
       <c r="K91" s="11">
-        <v>524.0</v>
+        <v>72.0</v>
       </c>
       <c r="L91" s="11">
-        <v>179.0</v>
+        <v>19.0</v>
       </c>
     </row>
     <row r="92">
       <c r="B92" s="13"/>
       <c r="E92" s="11">
-        <v>89.0</v>
+        <v>13.0</v>
       </c>
       <c r="F92" s="11">
-        <v>113.0</v>
+        <v>14.0</v>
       </c>
       <c r="G92" s="11">
-        <v>110.0</v>
+        <v>12.0</v>
       </c>
       <c r="H92" s="11">
-        <v>108.0</v>
+        <v>9.0</v>
       </c>
       <c r="I92" s="11">
-        <v>95.0</v>
+        <v>7.0</v>
       </c>
       <c r="J92" s="11">
-        <v>104.0</v>
+        <v>8.0</v>
       </c>
       <c r="K92" s="11">
-        <v>80.0</v>
+        <v>6.0</v>
       </c>
       <c r="L92" s="11">
-        <v>50.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="93">
       <c r="B93" s="13"/>
       <c r="E93" s="11">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
       <c r="F93" s="11">
-        <v>8.0</v>
+        <v>2.0</v>
       </c>
       <c r="G93" s="11">
-        <v>8.0</v>
+        <v>0.0</v>
       </c>
       <c r="H93" s="11">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
       <c r="I93" s="11">
-        <v>6.0</v>
+        <v>1.0</v>
       </c>
       <c r="J93" s="11">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="K93" s="11">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="L93" s="11">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="94">
@@ -6855,28 +6852,28 @@
         <v>23</v>
       </c>
       <c r="E95" s="11">
-        <v>133.0</v>
+        <v>13.0</v>
       </c>
       <c r="F95" s="11">
-        <v>68.0</v>
+        <v>10.0</v>
       </c>
       <c r="G95" s="11">
-        <v>17.0</v>
+        <v>1.0</v>
       </c>
       <c r="H95" s="11">
-        <v>28.0</v>
+        <v>6.0</v>
       </c>
       <c r="I95" s="11">
-        <v>40.0</v>
+        <v>6.0</v>
       </c>
       <c r="J95" s="11">
-        <v>137.0</v>
+        <v>26.0</v>
       </c>
       <c r="K95" s="11">
-        <v>405.0</v>
+        <v>77.0</v>
       </c>
       <c r="L95" s="11">
-        <v>1240.0</v>
+        <v>262.0</v>
       </c>
     </row>
     <row r="96">
@@ -6888,28 +6885,28 @@
         <v>25</v>
       </c>
       <c r="E96" s="11">
-        <v>303.0</v>
+        <v>27.0</v>
       </c>
       <c r="F96" s="11">
-        <v>224.0</v>
+        <v>21.0</v>
       </c>
       <c r="G96" s="11">
-        <v>138.0</v>
+        <v>13.0</v>
       </c>
       <c r="H96" s="11">
-        <v>101.0</v>
+        <v>10.0</v>
       </c>
       <c r="I96" s="11">
-        <v>127.0</v>
+        <v>16.0</v>
       </c>
       <c r="J96" s="11">
-        <v>235.0</v>
+        <v>31.0</v>
       </c>
       <c r="K96" s="11">
-        <v>288.0</v>
+        <v>42.0</v>
       </c>
       <c r="L96" s="11">
-        <v>774.0</v>
+        <v>122.0</v>
       </c>
     </row>
     <row r="97">
@@ -6955,55 +6952,55 @@
     <row r="99">
       <c r="B99" s="13"/>
       <c r="E99" s="11">
-        <v>3468.0</v>
+        <v>655.0</v>
       </c>
       <c r="F99" s="11">
-        <v>1562.0</v>
+        <v>176.0</v>
       </c>
       <c r="G99" s="11">
-        <v>1124.0</v>
+        <v>117.0</v>
       </c>
       <c r="H99" s="11">
-        <v>1219.0</v>
+        <v>156.0</v>
       </c>
       <c r="I99" s="11">
-        <v>2119.0</v>
+        <v>306.0</v>
       </c>
       <c r="J99" s="11">
-        <v>1854.0</v>
+        <v>252.0</v>
       </c>
       <c r="K99" s="11">
-        <v>1115.0</v>
+        <v>140.0</v>
       </c>
       <c r="L99" s="11">
-        <v>1170.0</v>
+        <v>135.0</v>
       </c>
     </row>
     <row r="100">
       <c r="B100" s="13"/>
       <c r="E100" s="11">
-        <v>1553.0</v>
+        <v>238.0</v>
       </c>
       <c r="F100" s="11">
-        <v>1345.0</v>
+        <v>206.0</v>
       </c>
       <c r="G100" s="11">
-        <v>1196.0</v>
+        <v>192.0</v>
       </c>
       <c r="H100" s="11">
-        <v>989.0</v>
+        <v>141.0</v>
       </c>
       <c r="I100" s="11">
-        <v>966.0</v>
+        <v>107.0</v>
       </c>
       <c r="J100" s="11">
-        <v>1022.0</v>
+        <v>128.0</v>
       </c>
       <c r="K100" s="11">
-        <v>1079.0</v>
+        <v>143.0</v>
       </c>
       <c r="L100" s="11">
-        <v>1176.0</v>
+        <v>129.0</v>
       </c>
     </row>
     <row r="101">
@@ -7047,55 +7044,55 @@
     <row r="103">
       <c r="B103" s="13"/>
       <c r="E103" s="11">
-        <v>1113.0</v>
+        <v>171.0</v>
       </c>
       <c r="F103" s="11">
-        <v>1783.0</v>
+        <v>358.0</v>
       </c>
       <c r="G103" s="11">
-        <v>1477.0</v>
+        <v>478.0</v>
       </c>
       <c r="H103" s="11">
-        <v>1021.0</v>
+        <v>179.0</v>
       </c>
       <c r="I103" s="11">
-        <v>893.0</v>
+        <v>161.0</v>
       </c>
       <c r="J103" s="11">
-        <v>747.0</v>
+        <v>125.0</v>
       </c>
       <c r="K103" s="11">
-        <v>621.0</v>
+        <v>93.0</v>
       </c>
       <c r="L103" s="11">
-        <v>359.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="104">
       <c r="B104" s="13"/>
       <c r="E104" s="11">
-        <v>1185.0</v>
+        <v>144.0</v>
       </c>
       <c r="F104" s="11">
-        <v>1200.0</v>
+        <v>206.0</v>
       </c>
       <c r="G104" s="11">
-        <v>742.0</v>
+        <v>159.0</v>
       </c>
       <c r="H104" s="11">
-        <v>567.0</v>
+        <v>98.0</v>
       </c>
       <c r="I104" s="11">
-        <v>575.0</v>
+        <v>90.0</v>
       </c>
       <c r="J104" s="11">
-        <v>526.0</v>
+        <v>62.0</v>
       </c>
       <c r="K104" s="11">
-        <v>418.0</v>
+        <v>52.0</v>
       </c>
       <c r="L104" s="11">
-        <v>329.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="105">
@@ -7153,28 +7150,28 @@
         <v>23</v>
       </c>
       <c r="E107" s="11">
-        <v>245.0</v>
+        <v>49.0</v>
       </c>
       <c r="F107" s="11">
-        <v>147.0</v>
+        <v>13.0</v>
       </c>
       <c r="G107" s="11">
-        <v>89.0</v>
+        <v>10.0</v>
       </c>
       <c r="H107" s="11">
-        <v>74.0</v>
+        <v>15.0</v>
       </c>
       <c r="I107" s="11">
-        <v>162.0</v>
+        <v>28.0</v>
       </c>
       <c r="J107" s="11">
-        <v>203.0</v>
+        <v>36.0</v>
       </c>
       <c r="K107" s="11">
-        <v>393.0</v>
+        <v>62.0</v>
       </c>
       <c r="L107" s="11">
-        <v>809.0</v>
+        <v>199.0</v>
       </c>
     </row>
     <row r="108">
@@ -7186,28 +7183,28 @@
         <v>25</v>
       </c>
       <c r="E108" s="11">
-        <v>384.0</v>
+        <v>38.0</v>
       </c>
       <c r="F108" s="11">
-        <v>289.0</v>
+        <v>27.0</v>
       </c>
       <c r="G108" s="11">
-        <v>201.0</v>
+        <v>11.0</v>
       </c>
       <c r="H108" s="11">
-        <v>138.0</v>
+        <v>8.0</v>
       </c>
       <c r="I108" s="11">
-        <v>193.0</v>
+        <v>26.0</v>
       </c>
       <c r="J108" s="11">
-        <v>321.0</v>
+        <v>45.0</v>
       </c>
       <c r="K108" s="11">
-        <v>523.0</v>
+        <v>102.0</v>
       </c>
       <c r="L108" s="11">
-        <v>786.0</v>
+        <v>166.0</v>
       </c>
     </row>
     <row r="109">
@@ -7253,55 +7250,55 @@
     <row r="111">
       <c r="B111" s="13"/>
       <c r="E111" s="11">
-        <v>1826.0</v>
+        <v>396.0</v>
       </c>
       <c r="F111" s="11">
-        <v>1376.0</v>
+        <v>240.0</v>
       </c>
       <c r="G111" s="11">
-        <v>1016.0</v>
+        <v>149.0</v>
       </c>
       <c r="H111" s="11">
-        <v>887.0</v>
+        <v>112.0</v>
       </c>
       <c r="I111" s="11">
-        <v>1437.0</v>
+        <v>161.0</v>
       </c>
       <c r="J111" s="11">
-        <v>1181.0</v>
+        <v>142.0</v>
       </c>
       <c r="K111" s="11">
-        <v>1110.0</v>
+        <v>147.0</v>
       </c>
       <c r="L111" s="11">
-        <v>1169.0</v>
+        <v>198.0</v>
       </c>
     </row>
     <row r="112">
       <c r="B112" s="13"/>
       <c r="E112" s="11">
-        <v>1305.0</v>
+        <v>262.0</v>
       </c>
       <c r="F112" s="11">
-        <v>1434.0</v>
+        <v>222.0</v>
       </c>
       <c r="G112" s="11">
-        <v>1236.0</v>
+        <v>175.0</v>
       </c>
       <c r="H112" s="11">
-        <v>1200.0</v>
+        <v>185.0</v>
       </c>
       <c r="I112" s="11">
-        <v>1195.0</v>
+        <v>153.0</v>
       </c>
       <c r="J112" s="11">
-        <v>1289.0</v>
+        <v>174.0</v>
       </c>
       <c r="K112" s="11">
-        <v>1400.0</v>
+        <v>204.0</v>
       </c>
       <c r="L112" s="11">
-        <v>1449.0</v>
+        <v>221.0</v>
       </c>
     </row>
     <row r="113">
@@ -7345,55 +7342,55 @@
     <row r="115">
       <c r="B115" s="13"/>
       <c r="E115" s="11">
-        <v>1386.0</v>
+        <v>201.0</v>
       </c>
       <c r="F115" s="11">
-        <v>1476.0</v>
+        <v>264.0</v>
       </c>
       <c r="G115" s="11">
-        <v>1569.0</v>
+        <v>335.0</v>
       </c>
       <c r="H115" s="11">
-        <v>1656.0</v>
+        <v>275.0</v>
       </c>
       <c r="I115" s="11">
-        <v>1357.0</v>
+        <v>255.0</v>
       </c>
       <c r="J115" s="11">
-        <v>1154.0</v>
+        <v>199.0</v>
       </c>
       <c r="K115" s="11">
-        <v>871.0</v>
+        <v>117.0</v>
       </c>
       <c r="L115" s="11">
-        <v>600.0</v>
+        <v>88.0</v>
       </c>
     </row>
     <row r="116">
       <c r="B116" s="13"/>
       <c r="E116" s="11">
-        <v>1590.0</v>
+        <v>211.0</v>
       </c>
       <c r="F116" s="11">
-        <v>1775.0</v>
+        <v>270.0</v>
       </c>
       <c r="G116" s="11">
-        <v>2114.0</v>
+        <v>340.0</v>
       </c>
       <c r="H116" s="11">
-        <v>1492.0</v>
+        <v>200.0</v>
       </c>
       <c r="I116" s="11">
-        <v>1027.0</v>
+        <v>109.0</v>
       </c>
       <c r="J116" s="11">
-        <v>797.0</v>
+        <v>107.0</v>
       </c>
       <c r="K116" s="11">
-        <v>665.0</v>
+        <v>89.0</v>
       </c>
       <c r="L116" s="11">
-        <v>492.0</v>
+        <v>72.0</v>
       </c>
     </row>
     <row r="117">
@@ -7451,7 +7448,7 @@
         <v>73</v>
       </c>
       <c r="E119" s="11">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="F119" s="11">
         <v>0.0</v>
@@ -7463,16 +7460,16 @@
         <v>0.0</v>
       </c>
       <c r="I119" s="11">
+        <v>0.0</v>
+      </c>
+      <c r="J119" s="11">
         <v>1.0</v>
       </c>
-      <c r="J119" s="11">
+      <c r="K119" s="11">
         <v>2.0</v>
       </c>
-      <c r="K119" s="11">
-        <v>31.0</v>
-      </c>
       <c r="L119" s="11">
-        <v>157.0</v>
+        <v>32.0</v>
       </c>
     </row>
     <row r="120">
@@ -7484,28 +7481,28 @@
         <v>25</v>
       </c>
       <c r="E120" s="11">
-        <v>19.0</v>
+        <v>2.0</v>
       </c>
       <c r="F120" s="11">
-        <v>7.0</v>
+        <v>0.0</v>
       </c>
       <c r="G120" s="11">
-        <v>6.0</v>
+        <v>1.0</v>
       </c>
       <c r="H120" s="11">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="I120" s="11">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="J120" s="11">
-        <v>11.0</v>
+        <v>4.0</v>
       </c>
       <c r="K120" s="11">
-        <v>145.0</v>
+        <v>31.0</v>
       </c>
       <c r="L120" s="11">
-        <v>252.0</v>
+        <v>54.0</v>
       </c>
     </row>
     <row r="121">
@@ -7551,55 +7548,55 @@
     <row r="123">
       <c r="B123" s="13"/>
       <c r="E123" s="11">
-        <v>264.0</v>
+        <v>47.0</v>
       </c>
       <c r="F123" s="11">
-        <v>127.0</v>
+        <v>7.0</v>
       </c>
       <c r="G123" s="11">
-        <v>128.0</v>
+        <v>9.0</v>
       </c>
       <c r="H123" s="11">
-        <v>220.0</v>
+        <v>26.0</v>
       </c>
       <c r="I123" s="11">
-        <v>295.0</v>
+        <v>23.0</v>
       </c>
       <c r="J123" s="11">
-        <v>218.0</v>
+        <v>12.0</v>
       </c>
       <c r="K123" s="11">
-        <v>96.0</v>
+        <v>8.0</v>
       </c>
       <c r="L123" s="11">
-        <v>307.0</v>
+        <v>37.0</v>
       </c>
     </row>
     <row r="124">
       <c r="B124" s="13"/>
       <c r="E124" s="11">
-        <v>313.0</v>
+        <v>68.0</v>
       </c>
       <c r="F124" s="11">
-        <v>344.0</v>
+        <v>53.0</v>
       </c>
       <c r="G124" s="11">
-        <v>292.0</v>
+        <v>41.0</v>
       </c>
       <c r="H124" s="11">
-        <v>167.0</v>
+        <v>45.0</v>
       </c>
       <c r="I124" s="11">
-        <v>179.0</v>
+        <v>32.0</v>
       </c>
       <c r="J124" s="11">
-        <v>212.0</v>
+        <v>25.0</v>
       </c>
       <c r="K124" s="11">
-        <v>301.0</v>
+        <v>37.0</v>
       </c>
       <c r="L124" s="11">
-        <v>319.0</v>
+        <v>38.0</v>
       </c>
     </row>
     <row r="125">
@@ -7643,55 +7640,55 @@
     <row r="127">
       <c r="B127" s="13"/>
       <c r="E127" s="11">
-        <v>214.0</v>
+        <v>37.0</v>
       </c>
       <c r="F127" s="11">
-        <v>223.0</v>
+        <v>36.0</v>
       </c>
       <c r="G127" s="11">
-        <v>285.0</v>
+        <v>73.0</v>
       </c>
       <c r="H127" s="11">
-        <v>213.0</v>
+        <v>74.0</v>
       </c>
       <c r="I127" s="11">
-        <v>59.0</v>
+        <v>4.0</v>
       </c>
       <c r="J127" s="11">
-        <v>187.0</v>
+        <v>45.0</v>
       </c>
       <c r="K127" s="11">
-        <v>249.0</v>
+        <v>44.0</v>
       </c>
       <c r="L127" s="11">
-        <v>6.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="128">
       <c r="B128" s="13"/>
       <c r="E128" s="11">
-        <v>461.0</v>
+        <v>93.0</v>
       </c>
       <c r="F128" s="11">
-        <v>251.0</v>
+        <v>59.0</v>
       </c>
       <c r="G128" s="11">
-        <v>133.0</v>
+        <v>20.0</v>
       </c>
       <c r="H128" s="11">
-        <v>71.0</v>
+        <v>18.0</v>
       </c>
       <c r="I128" s="11">
-        <v>69.0</v>
+        <v>15.0</v>
       </c>
       <c r="J128" s="11">
-        <v>58.0</v>
+        <v>5.0</v>
       </c>
       <c r="K128" s="11">
-        <v>48.0</v>
+        <v>10.0</v>
       </c>
       <c r="L128" s="11">
-        <v>12.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="129">
@@ -7749,28 +7746,28 @@
         <v>23</v>
       </c>
       <c r="E131" s="11">
-        <v>49.0</v>
+        <v>11.0</v>
       </c>
       <c r="F131" s="11">
-        <v>13.0</v>
+        <v>3.0</v>
       </c>
       <c r="G131" s="11">
-        <v>16.0</v>
+        <v>4.0</v>
       </c>
       <c r="H131" s="11">
-        <v>16.0</v>
+        <v>2.0</v>
       </c>
       <c r="I131" s="11">
-        <v>45.0</v>
+        <v>8.0</v>
       </c>
       <c r="J131" s="11">
-        <v>47.0</v>
+        <v>17.0</v>
       </c>
       <c r="K131" s="11">
-        <v>110.0</v>
+        <v>22.0</v>
       </c>
       <c r="L131" s="11">
-        <v>155.0</v>
+        <v>31.0</v>
       </c>
     </row>
     <row r="132">
@@ -7782,28 +7779,28 @@
         <v>25</v>
       </c>
       <c r="E132" s="11">
-        <v>259.0</v>
+        <v>38.0</v>
       </c>
       <c r="F132" s="11">
-        <v>162.0</v>
+        <v>20.0</v>
       </c>
       <c r="G132" s="11">
-        <v>150.0</v>
+        <v>22.0</v>
       </c>
       <c r="H132" s="11">
-        <v>124.0</v>
+        <v>11.0</v>
       </c>
       <c r="I132" s="11">
-        <v>163.0</v>
+        <v>17.0</v>
       </c>
       <c r="J132" s="11">
-        <v>328.0</v>
+        <v>51.0</v>
       </c>
       <c r="K132" s="11">
-        <v>622.0</v>
+        <v>110.0</v>
       </c>
       <c r="L132" s="11">
-        <v>860.0</v>
+        <v>142.0</v>
       </c>
     </row>
     <row r="133">
@@ -7849,55 +7846,55 @@
     <row r="135">
       <c r="B135" s="13"/>
       <c r="E135" s="11">
-        <v>296.0</v>
+        <v>59.0</v>
       </c>
       <c r="F135" s="11">
-        <v>335.0</v>
+        <v>49.0</v>
       </c>
       <c r="G135" s="11">
-        <v>343.0</v>
+        <v>72.0</v>
       </c>
       <c r="H135" s="11">
-        <v>428.0</v>
+        <v>57.0</v>
       </c>
       <c r="I135" s="11">
-        <v>363.0</v>
+        <v>37.0</v>
       </c>
       <c r="J135" s="11">
-        <v>400.0</v>
+        <v>71.0</v>
       </c>
       <c r="K135" s="11">
-        <v>425.0</v>
+        <v>65.0</v>
       </c>
       <c r="L135" s="11">
-        <v>516.0</v>
+        <v>66.0</v>
       </c>
     </row>
     <row r="136">
       <c r="B136" s="13"/>
       <c r="E136" s="11">
-        <v>1682.0</v>
+        <v>311.0</v>
       </c>
       <c r="F136" s="11">
-        <v>1488.0</v>
+        <v>237.0</v>
       </c>
       <c r="G136" s="11">
-        <v>1269.0</v>
+        <v>157.0</v>
       </c>
       <c r="H136" s="11">
-        <v>1156.0</v>
+        <v>170.0</v>
       </c>
       <c r="I136" s="11">
-        <v>1092.0</v>
+        <v>159.0</v>
       </c>
       <c r="J136" s="11">
-        <v>1166.0</v>
+        <v>140.0</v>
       </c>
       <c r="K136" s="11">
-        <v>1306.0</v>
+        <v>177.0</v>
       </c>
       <c r="L136" s="11">
-        <v>1481.0</v>
+        <v>194.0</v>
       </c>
     </row>
     <row r="137">
@@ -7941,55 +7938,55 @@
     <row r="139">
       <c r="B139" s="13"/>
       <c r="E139" s="11">
-        <v>515.0</v>
+        <v>78.0</v>
       </c>
       <c r="F139" s="11">
-        <v>334.0</v>
+        <v>49.0</v>
       </c>
       <c r="G139" s="11">
-        <v>352.0</v>
+        <v>48.0</v>
       </c>
       <c r="H139" s="11">
-        <v>275.0</v>
+        <v>41.0</v>
       </c>
       <c r="I139" s="11">
-        <v>239.0</v>
+        <v>41.0</v>
       </c>
       <c r="J139" s="11">
-        <v>226.0</v>
+        <v>27.0</v>
       </c>
       <c r="K139" s="11">
-        <v>139.0</v>
+        <v>20.0</v>
       </c>
       <c r="L139" s="11">
-        <v>76.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="140">
       <c r="B140" s="13"/>
       <c r="E140" s="11">
-        <v>1590.0</v>
+        <v>232.0</v>
       </c>
       <c r="F140" s="11">
-        <v>1811.0</v>
+        <v>273.0</v>
       </c>
       <c r="G140" s="11">
-        <v>1971.0</v>
+        <v>303.0</v>
       </c>
       <c r="H140" s="11">
-        <v>1531.0</v>
+        <v>240.0</v>
       </c>
       <c r="I140" s="11">
-        <v>1028.0</v>
+        <v>135.0</v>
       </c>
       <c r="J140" s="11">
-        <v>766.0</v>
+        <v>106.0</v>
       </c>
       <c r="K140" s="11">
-        <v>640.0</v>
+        <v>90.0</v>
       </c>
       <c r="L140" s="11">
-        <v>387.0</v>
+        <v>52.0</v>
       </c>
     </row>
     <row r="141">
@@ -8047,28 +8044,28 @@
         <v>23</v>
       </c>
       <c r="E143" s="11">
-        <v>25.0</v>
+        <v>7.0</v>
       </c>
       <c r="F143" s="11">
+        <v>2.0</v>
+      </c>
+      <c r="G143" s="11">
+        <v>2.0</v>
+      </c>
+      <c r="H143" s="11">
+        <v>1.0</v>
+      </c>
+      <c r="I143" s="11">
+        <v>2.0</v>
+      </c>
+      <c r="J143" s="11">
         <v>12.0</v>
       </c>
-      <c r="G143" s="11">
-        <v>10.0</v>
-      </c>
-      <c r="H143" s="11">
-        <v>6.0</v>
-      </c>
-      <c r="I143" s="11">
-        <v>24.0</v>
-      </c>
-      <c r="J143" s="11">
-        <v>53.0</v>
-      </c>
       <c r="K143" s="11">
-        <v>80.0</v>
+        <v>27.0</v>
       </c>
       <c r="L143" s="11">
-        <v>98.0</v>
+        <v>32.0</v>
       </c>
     </row>
     <row r="144">
@@ -8080,28 +8077,28 @@
         <v>25</v>
       </c>
       <c r="E144" s="11">
-        <v>319.0</v>
+        <v>48.0</v>
       </c>
       <c r="F144" s="11">
-        <v>235.0</v>
+        <v>27.0</v>
       </c>
       <c r="G144" s="11">
-        <v>196.0</v>
+        <v>25.0</v>
       </c>
       <c r="H144" s="11">
-        <v>161.0</v>
+        <v>13.0</v>
       </c>
       <c r="I144" s="11">
-        <v>201.0</v>
+        <v>28.0</v>
       </c>
       <c r="J144" s="11">
-        <v>342.0</v>
+        <v>50.0</v>
       </c>
       <c r="K144" s="11">
-        <v>613.0</v>
+        <v>120.0</v>
       </c>
       <c r="L144" s="11">
-        <v>938.0</v>
+        <v>174.0</v>
       </c>
     </row>
     <row r="145">
@@ -8147,55 +8144,55 @@
     <row r="147">
       <c r="B147" s="13"/>
       <c r="E147" s="11">
-        <v>212.0</v>
+        <v>51.0</v>
       </c>
       <c r="F147" s="11">
-        <v>360.0</v>
+        <v>91.0</v>
       </c>
       <c r="G147" s="11">
-        <v>339.0</v>
+        <v>55.0</v>
       </c>
       <c r="H147" s="11">
-        <v>316.0</v>
+        <v>68.0</v>
       </c>
       <c r="I147" s="11">
-        <v>285.0</v>
+        <v>45.0</v>
       </c>
       <c r="J147" s="11">
-        <v>304.0</v>
+        <v>45.0</v>
       </c>
       <c r="K147" s="11">
-        <v>297.0</v>
+        <v>64.0</v>
       </c>
       <c r="L147" s="11">
-        <v>339.0</v>
+        <v>35.0</v>
       </c>
     </row>
     <row r="148">
       <c r="B148" s="13"/>
       <c r="E148" s="11">
-        <v>1664.0</v>
+        <v>307.0</v>
       </c>
       <c r="F148" s="11">
-        <v>1482.0</v>
+        <v>229.0</v>
       </c>
       <c r="G148" s="11">
-        <v>1331.0</v>
+        <v>193.0</v>
       </c>
       <c r="H148" s="11">
-        <v>1223.0</v>
+        <v>189.0</v>
       </c>
       <c r="I148" s="11">
-        <v>1261.0</v>
+        <v>146.0</v>
       </c>
       <c r="J148" s="11">
-        <v>1251.0</v>
+        <v>161.0</v>
       </c>
       <c r="K148" s="11">
-        <v>1296.0</v>
+        <v>185.0</v>
       </c>
       <c r="L148" s="11">
-        <v>1432.0</v>
+        <v>201.0</v>
       </c>
     </row>
     <row r="149">
@@ -8239,55 +8236,55 @@
     <row r="151">
       <c r="B151" s="13"/>
       <c r="E151" s="11">
-        <v>308.0</v>
+        <v>70.0</v>
       </c>
       <c r="F151" s="11">
-        <v>265.0</v>
+        <v>48.0</v>
       </c>
       <c r="G151" s="11">
-        <v>181.0</v>
+        <v>36.0</v>
       </c>
       <c r="H151" s="11">
-        <v>162.0</v>
+        <v>32.0</v>
       </c>
       <c r="I151" s="11">
-        <v>99.0</v>
+        <v>18.0</v>
       </c>
       <c r="J151" s="11">
-        <v>78.0</v>
+        <v>22.0</v>
       </c>
       <c r="K151" s="11">
-        <v>84.0</v>
+        <v>9.0</v>
       </c>
       <c r="L151" s="11">
-        <v>51.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="152">
       <c r="B152" s="13"/>
       <c r="E152" s="11">
-        <v>1584.0</v>
+        <v>238.0</v>
       </c>
       <c r="F152" s="11">
-        <v>1800.0</v>
+        <v>252.0</v>
       </c>
       <c r="G152" s="11">
-        <v>2022.0</v>
+        <v>312.0</v>
       </c>
       <c r="H152" s="11">
-        <v>1570.0</v>
+        <v>243.0</v>
       </c>
       <c r="I152" s="11">
-        <v>985.0</v>
+        <v>151.0</v>
       </c>
       <c r="J152" s="11">
-        <v>873.0</v>
+        <v>111.0</v>
       </c>
       <c r="K152" s="11">
-        <v>733.0</v>
+        <v>107.0</v>
       </c>
       <c r="L152" s="11">
-        <v>473.0</v>
+        <v>64.0</v>
       </c>
     </row>
     <row r="153">
@@ -8345,61 +8342,61 @@
         <v>23</v>
       </c>
       <c r="E155" s="11">
-        <v>13.0</v>
+        <v>3.0</v>
       </c>
       <c r="F155" s="11">
-        <v>7.0</v>
+        <v>2.0</v>
       </c>
       <c r="G155" s="11">
+        <v>0.0</v>
+      </c>
+      <c r="H155" s="11">
+        <v>1.0</v>
+      </c>
+      <c r="I155" s="11">
+        <v>0.0</v>
+      </c>
+      <c r="J155" s="11">
         <v>3.0</v>
       </c>
-      <c r="H155" s="11">
-        <v>5.0</v>
-      </c>
-      <c r="I155" s="11">
-        <v>6.0</v>
-      </c>
-      <c r="J155" s="11">
-        <v>21.0</v>
-      </c>
       <c r="K155" s="11">
-        <v>29.0</v>
+        <v>3.0</v>
       </c>
       <c r="L155" s="11">
-        <v>20.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="156">
       <c r="B156" s="9"/>
       <c r="C156" s="10" t="s">
-        <v>83</v>
+        <v>50</v>
       </c>
       <c r="D156" s="10" t="s">
         <v>25</v>
       </c>
       <c r="E156" s="11">
-        <v>165.0</v>
+        <v>11.0</v>
       </c>
       <c r="F156" s="11">
-        <v>119.0</v>
+        <v>2.0</v>
       </c>
       <c r="G156" s="11">
-        <v>107.0</v>
+        <v>5.0</v>
       </c>
       <c r="H156" s="11">
-        <v>101.0</v>
+        <v>7.0</v>
       </c>
       <c r="I156" s="11">
-        <v>111.0</v>
+        <v>4.0</v>
       </c>
       <c r="J156" s="11">
-        <v>248.0</v>
+        <v>5.0</v>
       </c>
       <c r="K156" s="11">
-        <v>487.0</v>
+        <v>15.0</v>
       </c>
       <c r="L156" s="11">
-        <v>813.0</v>
+        <v>14.0</v>
       </c>
     </row>
     <row r="157">
@@ -8445,55 +8442,55 @@
     <row r="159">
       <c r="B159" s="13"/>
       <c r="E159" s="11">
-        <v>98.0</v>
+        <v>14.0</v>
       </c>
       <c r="F159" s="11">
-        <v>67.0</v>
+        <v>11.0</v>
       </c>
       <c r="G159" s="11">
-        <v>100.0</v>
+        <v>10.0</v>
       </c>
       <c r="H159" s="11">
-        <v>89.0</v>
+        <v>13.0</v>
       </c>
       <c r="I159" s="11">
-        <v>179.0</v>
+        <v>14.0</v>
       </c>
       <c r="J159" s="11">
-        <v>97.0</v>
+        <v>16.0</v>
       </c>
       <c r="K159" s="11">
-        <v>153.0</v>
+        <v>19.0</v>
       </c>
       <c r="L159" s="11">
-        <v>137.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="160">
       <c r="B160" s="13"/>
       <c r="E160" s="11">
-        <v>1026.0</v>
+        <v>21.0</v>
       </c>
       <c r="F160" s="11">
-        <v>1002.0</v>
+        <v>41.0</v>
       </c>
       <c r="G160" s="11">
-        <v>1107.0</v>
+        <v>37.0</v>
       </c>
       <c r="H160" s="11">
-        <v>1108.0</v>
+        <v>25.0</v>
       </c>
       <c r="I160" s="11">
-        <v>892.0</v>
+        <v>30.0</v>
       </c>
       <c r="J160" s="11">
-        <v>971.0</v>
+        <v>53.0</v>
       </c>
       <c r="K160" s="11">
-        <v>1042.0</v>
+        <v>43.0</v>
       </c>
       <c r="L160" s="11">
-        <v>1101.0</v>
+        <v>26.0</v>
       </c>
     </row>
     <row r="161">
@@ -8537,55 +8534,55 @@
     <row r="163">
       <c r="B163" s="13"/>
       <c r="E163" s="11">
-        <v>128.0</v>
+        <v>16.0</v>
       </c>
       <c r="F163" s="11">
-        <v>84.0</v>
+        <v>9.0</v>
       </c>
       <c r="G163" s="11">
-        <v>76.0</v>
+        <v>11.0</v>
       </c>
       <c r="H163" s="11">
-        <v>70.0</v>
+        <v>7.0</v>
       </c>
       <c r="I163" s="11">
-        <v>57.0</v>
+        <v>4.0</v>
       </c>
       <c r="J163" s="11">
-        <v>44.0</v>
+        <v>4.0</v>
       </c>
       <c r="K163" s="11">
-        <v>36.0</v>
+        <v>3.0</v>
       </c>
       <c r="L163" s="11">
-        <v>35.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="164">
       <c r="B164" s="13"/>
       <c r="E164" s="11">
-        <v>1261.0</v>
+        <v>36.0</v>
       </c>
       <c r="F164" s="11">
-        <v>1161.0</v>
+        <v>32.0</v>
       </c>
       <c r="G164" s="11">
-        <v>946.0</v>
+        <v>31.0</v>
       </c>
       <c r="H164" s="11">
-        <v>782.0</v>
+        <v>30.0</v>
       </c>
       <c r="I164" s="11">
-        <v>605.0</v>
+        <v>8.0</v>
       </c>
       <c r="J164" s="11">
-        <v>461.0</v>
+        <v>13.0</v>
       </c>
       <c r="K164" s="11">
-        <v>392.0</v>
+        <v>7.0</v>
       </c>
       <c r="L164" s="11">
-        <v>281.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="165">
@@ -8601,7 +8598,7 @@
     </row>
     <row r="166">
       <c r="B166" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C166" s="8" t="s">
         <v>12</v>
@@ -8637,67 +8634,67 @@
     <row r="167">
       <c r="B167" s="9"/>
       <c r="C167" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D167" s="10" t="s">
         <v>23</v>
       </c>
       <c r="E167" s="11">
-        <v>32.0</v>
+        <v>5.0</v>
       </c>
       <c r="F167" s="11">
+        <v>4.0</v>
+      </c>
+      <c r="G167" s="11">
+        <v>4.0</v>
+      </c>
+      <c r="H167" s="11">
+        <v>4.0</v>
+      </c>
+      <c r="I167" s="11">
+        <v>3.0</v>
+      </c>
+      <c r="J167" s="11">
         <v>11.0</v>
       </c>
-      <c r="G167" s="11">
-        <v>11.0</v>
-      </c>
-      <c r="H167" s="11">
-        <v>11.0</v>
-      </c>
-      <c r="I167" s="11">
-        <v>11.0</v>
-      </c>
-      <c r="J167" s="11">
-        <v>14.0</v>
-      </c>
       <c r="K167" s="11">
-        <v>18.0</v>
+        <v>5.0</v>
       </c>
       <c r="L167" s="11">
-        <v>45.0</v>
+        <v>26.0</v>
       </c>
     </row>
     <row r="168">
       <c r="B168" s="9"/>
       <c r="C168" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D168" s="10" t="s">
         <v>25</v>
       </c>
       <c r="E168" s="11">
-        <v>384.0</v>
+        <v>79.0</v>
       </c>
       <c r="F168" s="11">
-        <v>205.0</v>
+        <v>50.0</v>
       </c>
       <c r="G168" s="11">
-        <v>121.0</v>
+        <v>41.0</v>
       </c>
       <c r="H168" s="11">
-        <v>125.0</v>
+        <v>38.0</v>
       </c>
       <c r="I168" s="11">
-        <v>140.0</v>
+        <v>70.0</v>
       </c>
       <c r="J168" s="11">
-        <v>213.0</v>
+        <v>170.0</v>
       </c>
       <c r="K168" s="11">
-        <v>413.0</v>
+        <v>290.0</v>
       </c>
       <c r="L168" s="11">
-        <v>545.0</v>
+        <v>436.0</v>
       </c>
     </row>
     <row r="169">
@@ -8745,55 +8742,55 @@
     <row r="171">
       <c r="B171" s="13"/>
       <c r="E171" s="11">
-        <v>74.0</v>
+        <v>44.0</v>
       </c>
       <c r="F171" s="11">
-        <v>82.0</v>
+        <v>40.0</v>
       </c>
       <c r="G171" s="11">
-        <v>80.0</v>
+        <v>24.0</v>
       </c>
       <c r="H171" s="11">
-        <v>77.0</v>
+        <v>32.0</v>
       </c>
       <c r="I171" s="11">
-        <v>101.0</v>
+        <v>52.0</v>
       </c>
       <c r="J171" s="11">
-        <v>92.0</v>
+        <v>32.0</v>
       </c>
       <c r="K171" s="11">
-        <v>105.0</v>
+        <v>38.0</v>
       </c>
       <c r="L171" s="11">
-        <v>94.0</v>
+        <v>49.0</v>
       </c>
     </row>
     <row r="172">
       <c r="B172" s="13"/>
       <c r="E172" s="11">
-        <v>1237.0</v>
+        <v>498.0</v>
       </c>
       <c r="F172" s="11">
-        <v>1780.0</v>
+        <v>517.0</v>
       </c>
       <c r="G172" s="11">
-        <v>1825.0</v>
+        <v>432.0</v>
       </c>
       <c r="H172" s="11">
-        <v>1573.0</v>
+        <v>365.0</v>
       </c>
       <c r="I172" s="11">
-        <v>1577.0</v>
+        <v>345.0</v>
       </c>
       <c r="J172" s="11">
-        <v>1751.0</v>
+        <v>382.0</v>
       </c>
       <c r="K172" s="11">
-        <v>1697.0</v>
+        <v>457.0</v>
       </c>
       <c r="L172" s="11">
-        <v>1744.0</v>
+        <v>459.0</v>
       </c>
     </row>
     <row r="173">
@@ -8837,55 +8834,55 @@
     <row r="175">
       <c r="B175" s="13"/>
       <c r="E175" s="11">
-        <v>119.0</v>
+        <v>45.0</v>
       </c>
       <c r="F175" s="11">
-        <v>87.0</v>
+        <v>52.0</v>
       </c>
       <c r="G175" s="11">
-        <v>65.0</v>
+        <v>42.0</v>
       </c>
       <c r="H175" s="11">
-        <v>25.0</v>
+        <v>52.0</v>
       </c>
       <c r="I175" s="11">
+        <v>23.0</v>
+      </c>
+      <c r="J175" s="11">
         <v>34.0</v>
       </c>
-      <c r="J175" s="11">
-        <v>30.0</v>
-      </c>
       <c r="K175" s="11">
-        <v>23.0</v>
+        <v>29.0</v>
       </c>
       <c r="L175" s="11">
-        <v>35.0</v>
+        <v>19.0</v>
       </c>
     </row>
     <row r="176">
       <c r="B176" s="13"/>
       <c r="E176" s="11">
-        <v>1659.0</v>
+        <v>481.0</v>
       </c>
       <c r="F176" s="11">
-        <v>1602.0</v>
+        <v>512.0</v>
       </c>
       <c r="G176" s="11">
-        <v>1204.0</v>
+        <v>499.0</v>
       </c>
       <c r="H176" s="11">
-        <v>698.0</v>
+        <v>383.0</v>
       </c>
       <c r="I176" s="11">
-        <v>698.0</v>
+        <v>291.0</v>
       </c>
       <c r="J176" s="11">
-        <v>470.0</v>
+        <v>233.0</v>
       </c>
       <c r="K176" s="11">
-        <v>398.0</v>
+        <v>197.0</v>
       </c>
       <c r="L176" s="11">
-        <v>267.0</v>
+        <v>133.0</v>
       </c>
     </row>
     <row r="177">
@@ -9565,7 +9562,7 @@
     </row>
     <row r="362">
       <c r="B362" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C362" s="16" t="s">
         <v>23</v>

</xml_diff>